<commit_message>
feat: vcf formats support (#9)
* feat: add vcf and bcf to DataFormat enumeration

* chore: regen
</commit_message>
<xml_diff>
--- a/project/excel/modo_schema.xlsx
+++ b/project/excel/modo_schema.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="MODO" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Assay" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Sample" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="DataEntity" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="ReferenceGenome" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="ReferenceSequence" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="AlignmentSet" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="VariantSet" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Array" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="MODOCollection" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MODO" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Assay" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sample" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="DataEntity" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ReferenceGenome" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ReferenceSequence" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="AlignmentSet" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="VariantSet" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Array" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="MODOCollection" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -507,7 +507,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CRAM,FASTQ,Zarr,FASTA"</formula1>
+      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -772,7 +772,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CRAM,FASTQ,Zarr,FASTA"</formula1>
+      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -945,7 +945,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CRAM,FASTQ,Zarr,FASTA"</formula1>
+      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1006,7 +1006,7 @@
   </sheetData>
   <dataValidations count="1">
     <dataValidation sqref="B2:B1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"CRAM,FASTQ,Zarr,FASTA"</formula1>
+      <formula1>"CRAM,FASTQ,Zarr,FASTA,VCF,BCF"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>